<commit_message>
included db connection method
included db connection method
</commit_message>
<xml_diff>
--- a/Automation_Testdata/Testdata.xlsx
+++ b/Automation_Testdata/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t>Topupamount</t>
   </si>
@@ -60,16 +60,40 @@
     <t>cardPAN</t>
   </si>
   <si>
-    <t>308425310825581</t>
-  </si>
-  <si>
-    <t>308425027238516</t>
-  </si>
-  <si>
     <t>rambo</t>
   </si>
   <si>
     <t>xyz</t>
+  </si>
+  <si>
+    <t>847</t>
+  </si>
+  <si>
+    <t>308425000659399</t>
+  </si>
+  <si>
+    <t>308425000659407</t>
+  </si>
+  <si>
+    <t>308425000659449</t>
+  </si>
+  <si>
+    <t>308425000660017</t>
+  </si>
+  <si>
+    <t>308425000660074</t>
+  </si>
+  <si>
+    <t>308425000660108</t>
+  </si>
+  <si>
+    <t>308425000660462</t>
+  </si>
+  <si>
+    <t>308425000660645</t>
+  </si>
+  <si>
+    <t>308425000660652</t>
   </si>
 </sst>
 </file>
@@ -414,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,16 +487,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>4564</v>
@@ -492,22 +516,22 @@
       <c r="J2">
         <v>2019</v>
       </c>
-      <c r="K2">
-        <v>847</v>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>4564</v>
@@ -527,8 +551,253 @@
       <c r="J3">
         <v>2019</v>
       </c>
-      <c r="K3">
-        <v>847</v>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>4564</v>
+      </c>
+      <c r="F4">
+        <v>7100</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>2019</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>4564</v>
+      </c>
+      <c r="F5">
+        <v>7100</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>2019</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>4564</v>
+      </c>
+      <c r="F6">
+        <v>7100</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>2019</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>4564</v>
+      </c>
+      <c r="F7">
+        <v>7100</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>2019</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>4564</v>
+      </c>
+      <c r="F8">
+        <v>7100</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>2019</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>4564</v>
+      </c>
+      <c r="F9">
+        <v>7100</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>2019</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>4564</v>
+      </c>
+      <c r="F10">
+        <v>7100</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>2019</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
publish on november 1
includes code to identify settlement xml
</commit_message>
<xml_diff>
--- a/Automation_Testdata/Testdata.xlsx
+++ b/Automation_Testdata/Testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="carddetails" sheetId="1" r:id="rId2"/>
+    <sheet name="epass" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>Topupamount</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>308425000660652</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Zonemin</t>
+  </si>
+  <si>
+    <t>Zonemax</t>
+  </si>
+  <si>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Zone 2</t>
+  </si>
+  <si>
+    <t>308425030316432</t>
   </si>
 </sst>
 </file>
@@ -438,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +468,7 @@
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -484,8 +502,17 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -519,8 +546,17 @@
       <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>7</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -554,8 +590,17 @@
       <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -589,8 +634,17 @@
       <c r="K4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>7</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -624,8 +678,17 @@
       <c r="K5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -659,8 +722,17 @@
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>7</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -694,8 +766,17 @@
       <c r="K7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -729,8 +810,17 @@
       <c r="K8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -764,8 +854,17 @@
       <c r="K9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -798,6 +897,15 @@
       </c>
       <c r="K10" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -808,10 +916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:A5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,11 +929,75 @@
     <col min="3" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>4564</v>
+      </c>
+      <c r="F2">
+        <v>7100</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>2019</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>